<commit_message>
Update documentation and enhance content for February Heritage Happenings newsletter
</commit_message>
<xml_diff>
--- a/3-1-heritage/0-heritage-happenings/2025/02-february-hh/residents-directory/2025-02-heritage-resident-directory.xlsx
+++ b/3-1-heritage/0-heritage-happenings/2025/02-february-hh/residents-directory/2025-02-heritage-resident-directory.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4348e1419f457eb2/Documents/GitHub/theo-armour-agenda/3-1-heritage/0-heritage-happenings/2025/01-january-hh/resident-directory/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4348e1419f457eb2/Documents/GitHub/theo-armour-agenda/3-1-heritage/0-heritage-happenings/2025/02-february-hh/residents-directory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="802" documentId="8_{47523533-A004-48EF-BEEC-0FA3DE3C4717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88DF0510-77BC-4C86-9FE7-DF0D8C4147D0}"/>
+  <xr:revisionPtr revIDLastSave="805" documentId="8_{47523533-A004-48EF-BEEC-0FA3DE3C4717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D8EE3F8-3BA1-43D3-8E4B-73AF6156FD75}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="754" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="754" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="residents" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1677" uniqueCount="1092">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1678" uniqueCount="1092">
   <si>
     <t>First Name</t>
   </si>
@@ -3953,10 +3953,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -4161,9 +4157,9 @@
   </sheetPr>
   <dimension ref="A1:I1006"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.15234375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4368,7 +4364,9 @@
       <c r="B8" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="3"/>
+      <c r="C8" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="D8" s="1" t="s">
         <v>50</v>
       </c>
@@ -4378,9 +4376,7 @@
       <c r="F8" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>53</v>
-      </c>
+      <c r="G8" s="1"/>
       <c r="I8" s="4" t="s">
         <v>54</v>
       </c>
@@ -4392,7 +4388,9 @@
       <c r="B9" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="D9" s="1" t="s">
         <v>50</v>
       </c>
@@ -8888,7 +8886,7 @@
       <c r="I1006" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:H7 I2:AA19 C8:D9 F8:H9 C10:H11 C12:E13 G12:H13 C14:H19 C20:AA77">
+  <conditionalFormatting sqref="C2:H7 I2:AA19 F8:H9 C10:H11 C12:E13 G12:H13 C14:H19 C20:AA77 C8:D9">
     <cfRule type="expression" dxfId="18" priority="1">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
@@ -9726,7 +9724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26C4F1CA-A107-47E1-B61D-684F7BB5060E}">
   <dimension ref="A1:Z173"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" showRuler="0" view="pageLayout" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" showZeros="0" showRuler="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Remove outdated articles and update newsletter content for February Heritage Happenings
</commit_message>
<xml_diff>
--- a/3-1-heritage/0-heritage-happenings/2025/02-february-hh/residents-directory/2025-02-heritage-resident-directory.xlsx
+++ b/3-1-heritage/0-heritage-happenings/2025/02-february-hh/residents-directory/2025-02-heritage-resident-directory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4348e1419f457eb2/Documents/GitHub/theo-armour-agenda/3-1-heritage/0-heritage-happenings/2025/02-february-hh/residents-directory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="805" documentId="8_{47523533-A004-48EF-BEEC-0FA3DE3C4717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D8EE3F8-3BA1-43D3-8E4B-73AF6156FD75}"/>
+  <xr:revisionPtr revIDLastSave="807" documentId="8_{47523533-A004-48EF-BEEC-0FA3DE3C4717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E43E5195-7A6B-47B0-9017-E87EB37E4A41}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="754" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="754" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="residents" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -3703,7 +3703,6 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -3726,6 +3725,7 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="35" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="35" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="35" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3953,6 +3953,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -4157,7 +4161,7 @@
   </sheetPr>
   <dimension ref="A1:I1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
@@ -4169,7 +4173,7 @@
     <col min="3" max="3" width="9.15234375" style="17" customWidth="1"/>
     <col min="4" max="4" width="14.4609375" style="17" customWidth="1"/>
     <col min="5" max="5" width="13.4609375" style="17" customWidth="1"/>
-    <col min="6" max="6" width="26.4609375" style="40" customWidth="1"/>
+    <col min="6" max="6" width="26.4609375" style="39" customWidth="1"/>
     <col min="7" max="8" width="10.4609375" style="17" customWidth="1"/>
     <col min="9" max="9" width="7.15234375" style="17" customWidth="1"/>
     <col min="10" max="16384" width="11.15234375" style="17"/>
@@ -4191,7 +4195,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="F1" s="39" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -4220,7 +4224,7 @@
       <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="39" t="s">
         <v>14</v>
       </c>
       <c r="G2" s="3"/>
@@ -4273,7 +4277,7 @@
       <c r="E4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="40" t="s">
+      <c r="F4" s="39" t="s">
         <v>28</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -4300,7 +4304,7 @@
       <c r="E5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="40" t="s">
+      <c r="F5" s="39" t="s">
         <v>34</v>
       </c>
       <c r="G5" s="3" t="s">
@@ -4327,7 +4331,7 @@
       <c r="E6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="40" t="s">
+      <c r="F6" s="39" t="s">
         <v>40</v>
       </c>
       <c r="I6" s="4" t="s">
@@ -4350,7 +4354,7 @@
       <c r="E7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="40" t="s">
+      <c r="F7" s="39" t="s">
         <v>46</v>
       </c>
       <c r="I7" s="4" t="s">
@@ -4373,7 +4377,7 @@
       <c r="E8" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="40" t="s">
+      <c r="F8" s="39" t="s">
         <v>52</v>
       </c>
       <c r="G8" s="1"/>
@@ -4397,7 +4401,7 @@
       <c r="E9" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="40" t="s">
+      <c r="F9" s="39" t="s">
         <v>52</v>
       </c>
       <c r="G9" s="1" t="s">
@@ -4423,7 +4427,7 @@
       <c r="E10" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F10" s="40" t="s">
+      <c r="F10" s="39" t="s">
         <v>61</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -4450,7 +4454,7 @@
       <c r="E11" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F11" s="40" t="s">
+      <c r="F11" s="39" t="s">
         <v>67</v>
       </c>
       <c r="G11" s="1"/>
@@ -4546,7 +4550,7 @@
       <c r="E15" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F15" s="41" t="s">
+      <c r="F15" s="40" t="s">
         <v>89</v>
       </c>
       <c r="G15" s="3" t="s">
@@ -4573,7 +4577,7 @@
       <c r="E16" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F16" s="42" t="s">
+      <c r="F16" s="41" t="s">
         <v>93</v>
       </c>
       <c r="G16" s="1"/>
@@ -4600,7 +4604,7 @@
       <c r="E17" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F17" s="40" t="s">
+      <c r="F17" s="39" t="s">
         <v>98</v>
       </c>
       <c r="G17" s="3"/>
@@ -4650,7 +4654,7 @@
       <c r="E19" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F19" s="40" t="s">
+      <c r="F19" s="39" t="s">
         <v>109</v>
       </c>
       <c r="I19" s="4" t="s">
@@ -4673,7 +4677,7 @@
       <c r="E20" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F20" s="40" t="s">
+      <c r="F20" s="39" t="s">
         <v>115</v>
       </c>
       <c r="G20" s="1" t="s">
@@ -4699,7 +4703,7 @@
       <c r="E21" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="F21" s="40" t="s">
+      <c r="F21" s="39" t="s">
         <v>121</v>
       </c>
       <c r="G21" s="3" t="s">
@@ -4726,7 +4730,7 @@
       <c r="E22" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="F22" s="40" t="s">
+      <c r="F22" s="39" t="s">
         <v>126</v>
       </c>
       <c r="G22" s="3" t="s">
@@ -4753,7 +4757,7 @@
       <c r="E23" s="1" t="s">
         <v>1025</v>
       </c>
-      <c r="F23" s="41" t="s">
+      <c r="F23" s="40" t="s">
         <v>1027</v>
       </c>
       <c r="G23" s="3"/>
@@ -4801,7 +4805,7 @@
       <c r="E25" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="F25" s="40" t="s">
+      <c r="F25" s="39" t="s">
         <v>134</v>
       </c>
       <c r="G25" s="1" t="s">
@@ -4828,7 +4832,7 @@
       <c r="E26" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="F26" s="41" t="s">
+      <c r="F26" s="40" t="s">
         <v>140</v>
       </c>
       <c r="G26" s="1" t="s">
@@ -4857,7 +4861,7 @@
       <c r="E27" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="F27" s="40" t="s">
+      <c r="F27" s="39" t="s">
         <v>146</v>
       </c>
       <c r="G27" s="1" t="s">
@@ -4934,7 +4938,7 @@
       <c r="E30" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="F30" s="40" t="s">
+      <c r="F30" s="39" t="s">
         <v>159</v>
       </c>
       <c r="G30" s="3"/>
@@ -4959,7 +4963,7 @@
       <c r="E31" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="F31" s="40" t="s">
+      <c r="F31" s="39" t="s">
         <v>165</v>
       </c>
       <c r="G31" s="3" t="s">
@@ -4986,7 +4990,7 @@
       <c r="E32" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="F32" s="40" t="s">
+      <c r="F32" s="39" t="s">
         <v>170</v>
       </c>
       <c r="G32" s="3" t="s">
@@ -5035,7 +5039,7 @@
       <c r="E34" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="F34" s="40" t="s">
+      <c r="F34" s="39" t="s">
         <v>180</v>
       </c>
       <c r="G34" s="1"/>
@@ -5062,7 +5066,7 @@
       <c r="E35" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="F35" s="40" t="s">
+      <c r="F35" s="39" t="s">
         <v>186</v>
       </c>
       <c r="I35" s="4" t="s">
@@ -5085,7 +5089,7 @@
       <c r="E36" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="F36" s="41" t="s">
+      <c r="F36" s="40" t="s">
         <v>192</v>
       </c>
       <c r="I36" s="4" t="s">
@@ -5108,7 +5112,7 @@
       <c r="E37" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="F37" s="40" t="s">
+      <c r="F37" s="39" t="s">
         <v>198</v>
       </c>
       <c r="I37" s="4" t="s">
@@ -5131,7 +5135,7 @@
       <c r="E38" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="F38" s="40" t="s">
+      <c r="F38" s="39" t="s">
         <v>203</v>
       </c>
       <c r="G38" s="1" t="s">
@@ -5204,7 +5208,7 @@
       <c r="E41" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="F41" s="40" t="s">
+      <c r="F41" s="39" t="s">
         <v>219</v>
       </c>
       <c r="I41" s="4" t="s">
@@ -5227,7 +5231,7 @@
       <c r="E42" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="F42" s="40" t="s">
+      <c r="F42" s="39" t="s">
         <v>219</v>
       </c>
       <c r="G42" s="3"/>
@@ -5254,7 +5258,7 @@
       <c r="E43" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="F43" s="40" t="s">
+      <c r="F43" s="39" t="s">
         <v>228</v>
       </c>
       <c r="G43" s="3"/>
@@ -5279,7 +5283,7 @@
       <c r="E44" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="F44" s="41" t="s">
+      <c r="F44" s="40" t="s">
         <v>234</v>
       </c>
       <c r="G44" s="1" t="s">
@@ -5305,7 +5309,7 @@
       <c r="E45" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="F45" s="40" t="s">
+      <c r="F45" s="39" t="s">
         <v>238</v>
       </c>
       <c r="G45" s="1"/>
@@ -5330,7 +5334,7 @@
       <c r="E46" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="F46" s="40" t="s">
+      <c r="F46" s="39" t="s">
         <v>244</v>
       </c>
       <c r="G46" s="1" t="s">
@@ -5401,7 +5405,7 @@
       <c r="E49" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="F49" s="40" t="s">
+      <c r="F49" s="39" t="s">
         <v>258</v>
       </c>
       <c r="I49" s="4" t="s">
@@ -5424,7 +5428,7 @@
       <c r="E50" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="F50" s="40" t="s">
+      <c r="F50" s="39" t="s">
         <v>264</v>
       </c>
       <c r="I50" s="4" t="s">
@@ -5447,7 +5451,7 @@
       <c r="E51" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="F51" s="40" t="s">
+      <c r="F51" s="39" t="s">
         <v>269</v>
       </c>
       <c r="G51" s="1"/>
@@ -5472,7 +5476,7 @@
       <c r="E52" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="F52" s="40" t="s">
+      <c r="F52" s="39" t="s">
         <v>275</v>
       </c>
       <c r="G52" s="1" t="s">
@@ -5519,7 +5523,7 @@
       <c r="E54" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="F54" s="40" t="s">
+      <c r="F54" s="39" t="s">
         <v>286</v>
       </c>
       <c r="G54" s="1" t="s">
@@ -5546,7 +5550,7 @@
       <c r="E55" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="F55" s="40" t="s">
+      <c r="F55" s="39" t="s">
         <v>290</v>
       </c>
       <c r="G55" s="3" t="s">
@@ -5575,7 +5579,7 @@
       <c r="E56" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="F56" s="50" t="s">
+      <c r="F56" s="49" t="s">
         <v>1082</v>
       </c>
       <c r="G56" s="1"/>
@@ -5600,7 +5604,7 @@
       <c r="E57" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="F57" s="40" t="s">
+      <c r="F57" s="39" t="s">
         <v>298</v>
       </c>
       <c r="I57" s="4" t="s">
@@ -5623,7 +5627,7 @@
       <c r="E58" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="F58" s="40" t="s">
+      <c r="F58" s="39" t="s">
         <v>304</v>
       </c>
       <c r="I58" s="4" t="s">
@@ -5670,7 +5674,7 @@
       <c r="E60" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="F60" s="40" t="s">
+      <c r="F60" s="39" t="s">
         <v>315</v>
       </c>
       <c r="H60" s="1" t="s">
@@ -5745,7 +5749,7 @@
       <c r="E63" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="F63" s="40" t="s">
+      <c r="F63" s="39" t="s">
         <v>330</v>
       </c>
       <c r="G63" s="1"/>
@@ -5770,7 +5774,7 @@
       <c r="E64" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="F64" s="40" t="s">
+      <c r="F64" s="39" t="s">
         <v>335</v>
       </c>
       <c r="G64" s="1" t="s">
@@ -5797,7 +5801,7 @@
       <c r="E65" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="F65" s="40" t="s">
+      <c r="F65" s="39" t="s">
         <v>339</v>
       </c>
       <c r="G65" s="1"/>
@@ -5822,7 +5826,7 @@
       <c r="E66" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="F66" s="40" t="s">
+      <c r="F66" s="39" t="s">
         <v>345</v>
       </c>
       <c r="G66" s="1" t="s">
@@ -5848,7 +5852,7 @@
       <c r="E67" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="F67" s="40" t="s">
+      <c r="F67" s="39" t="s">
         <v>350</v>
       </c>
       <c r="G67" s="1"/>
@@ -5872,7 +5876,7 @@
       <c r="E68" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="F68" s="40" t="s">
+      <c r="F68" s="39" t="s">
         <v>354</v>
       </c>
       <c r="G68" s="1"/>
@@ -5897,7 +5901,7 @@
       <c r="E69" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="F69" s="40" t="s">
+      <c r="F69" s="39" t="s">
         <v>358</v>
       </c>
       <c r="I69" s="4" t="s">
@@ -5920,7 +5924,7 @@
       <c r="E70" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="F70" s="41" t="s">
+      <c r="F70" s="40" t="s">
         <v>363</v>
       </c>
       <c r="I70" s="4" t="s">
@@ -5943,7 +5947,7 @@
       <c r="E71" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="F71" s="40" t="s">
+      <c r="F71" s="39" t="s">
         <v>368</v>
       </c>
       <c r="I71" s="17" t="s">
@@ -6013,7 +6017,7 @@
       <c r="E74" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="F74" s="40" t="s">
+      <c r="F74" s="39" t="s">
         <v>383</v>
       </c>
       <c r="G74" s="1" t="s">
@@ -6040,7 +6044,7 @@
       <c r="E75" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="F75" s="40" t="s">
+      <c r="F75" s="39" t="s">
         <v>388</v>
       </c>
       <c r="G75" s="1"/>
@@ -6065,7 +6069,7 @@
       <c r="E76" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="F76" s="43"/>
+      <c r="F76" s="42"/>
       <c r="G76" s="3" t="s">
         <v>53</v>
       </c>
@@ -8886,7 +8890,7 @@
       <c r="I1006" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:H7 I2:AA19 F8:H9 C10:H11 C12:E13 G12:H13 C14:H19 C20:AA77 C8:D9">
+  <conditionalFormatting sqref="C2:H7 I2:AA19 C8:D9 F8:H9 C10:H11 C12:E13 G12:H13 C14:H19 C20:AA77">
     <cfRule type="expression" dxfId="18" priority="1">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
@@ -9144,7 +9148,7 @@
       <c r="E10" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="F10" s="40"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="4" t="s">
@@ -9217,7 +9221,7 @@
       <c r="E13" s="1" t="s">
         <v>547</v>
       </c>
-      <c r="F13" s="40" t="s">
+      <c r="F13" s="39" t="s">
         <v>548</v>
       </c>
       <c r="G13" s="3" t="s">
@@ -9724,8 +9728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26C4F1CA-A107-47E1-B61D-684F7BB5060E}">
   <dimension ref="A1:Z173"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" showRuler="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83"/>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" showRuler="0" view="pageLayout" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.765625" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -9778,19 +9782,19 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="53" t="str">
+      <c r="A3" s="52" t="str">
         <v>Barbara Anderson</v>
       </c>
-      <c r="B3" s="53" t="str">
+      <c r="B3" s="52" t="str">
         <v>422 P</v>
       </c>
-      <c r="C3" s="53" t="str">
+      <c r="C3" s="52" t="str">
         <v>415-244-4882</v>
       </c>
-      <c r="D3" s="53">
+      <c r="D3" s="52">
         <v>0</v>
       </c>
-      <c r="E3" s="53" t="str">
+      <c r="E3" s="52" t="str">
         <v>09/10</v>
       </c>
     </row>
@@ -9930,20 +9934,20 @@
         <v>07/15</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="52" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="54" t="str">
+    <row r="12" spans="1:5" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="53" t="str">
         <v>Harry Copeland</v>
       </c>
-      <c r="B12" s="54" t="str">
+      <c r="B12" s="53" t="str">
         <v>121 P</v>
       </c>
-      <c r="C12" s="54" t="str">
+      <c r="C12" s="53" t="str">
         <v>415 673-2884</v>
       </c>
-      <c r="D12" s="54">
+      <c r="D12" s="53">
         <v>0</v>
       </c>
-      <c r="E12" s="54" t="str">
+      <c r="E12" s="53" t="str">
         <v>04/01</v>
       </c>
     </row>
@@ -10118,19 +10122,19 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="44" t="str">
+      <c r="A23" s="43" t="str">
         <v>Cooby Greenway</v>
       </c>
-      <c r="B23" s="44" t="str">
+      <c r="B23" s="43" t="str">
         <v>1530 Francisco</v>
       </c>
-      <c r="C23" s="44" t="str">
+      <c r="C23" s="43" t="str">
         <v>202 320-4577</v>
       </c>
-      <c r="D23" s="44" t="str">
+      <c r="D23" s="43" t="str">
         <v>cgreenway2804@gmail.com</v>
       </c>
-      <c r="E23" s="44" t="str">
+      <c r="E23" s="43" t="str">
         <v>02/06</v>
       </c>
     </row>
@@ -10645,19 +10649,19 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="38" t="str">
+      <c r="A54" s="54" t="str">
         <v>Kay Narron</v>
       </c>
-      <c r="B54" s="38" t="str">
+      <c r="B54" s="54" t="str">
         <v>418 P</v>
       </c>
-      <c r="C54" s="38" t="str">
+      <c r="C54" s="54" t="str">
         <v>530 401-8491</v>
       </c>
-      <c r="D54" s="38" t="str">
+      <c r="D54" s="54" t="str">
         <v>kay.narron@gmail.com</v>
       </c>
-      <c r="E54" s="38" t="str">
+      <c r="E54" s="54" t="str">
         <v>01/04</v>
       </c>
     </row>
@@ -10781,19 +10785,19 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62" s="54" t="str">
+      <c r="A62" s="53" t="str">
         <v>Robert Segrin</v>
       </c>
-      <c r="B62" s="54" t="str">
+      <c r="B62" s="53" t="str">
         <v>121 P</v>
       </c>
-      <c r="C62" s="54" t="str">
+      <c r="C62" s="53" t="str">
         <v>415 673-1333</v>
       </c>
-      <c r="D62" s="54">
+      <c r="D62" s="53">
         <v>0</v>
       </c>
-      <c r="E62" s="54" t="str">
+      <c r="E62" s="53" t="str">
         <v>08/23</v>
       </c>
     </row>
@@ -11019,36 +11023,36 @@
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A76" s="52" t="str">
+      <c r="A76" s="51" t="str">
         <v>Shirley Yawitz</v>
       </c>
-      <c r="B76" s="52" t="str">
+      <c r="B76" s="51" t="str">
         <v>246 M</v>
       </c>
-      <c r="C76" s="52" t="str">
+      <c r="C76" s="51" t="str">
         <v>415 929-6992</v>
       </c>
-      <c r="D76" s="52">
+      <c r="D76" s="51">
         <v>0</v>
       </c>
-      <c r="E76" s="52" t="str">
+      <c r="E76" s="51" t="str">
         <v>-</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A77" s="53" t="str">
+      <c r="A77" s="52" t="str">
         <v>Flora Zagorites</v>
       </c>
-      <c r="B77" s="53" t="str">
+      <c r="B77" s="52" t="str">
         <v>238 M</v>
       </c>
-      <c r="C77" s="53" t="str">
+      <c r="C77" s="52" t="str">
         <v>415 710-2771</v>
       </c>
-      <c r="D77" s="53">
+      <c r="D77" s="52">
         <v>0</v>
       </c>
-      <c r="E77" s="53" t="str">
+      <c r="E77" s="52" t="str">
         <v>02/16</v>
       </c>
     </row>
@@ -11072,13 +11076,13 @@
       <c r="E81" s="24"/>
     </row>
     <row r="82" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A82" s="53" t="s">
+      <c r="A82" s="52" t="s">
         <v>1091</v>
       </c>
-      <c r="B82" s="53"/>
-      <c r="C82" s="53"/>
-      <c r="D82" s="53"/>
-      <c r="E82" s="53"/>
+      <c r="B82" s="52"/>
+      <c r="C82" s="52"/>
+      <c r="D82" s="52"/>
+      <c r="E82" s="52"/>
     </row>
     <row r="84" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A84" s="13" t="s">
@@ -11789,7 +11793,7 @@
         <v>473</v>
       </c>
       <c r="C107" s="37"/>
-      <c r="D107" s="39" t="s">
+      <c r="D107" s="38" t="s">
         <v>474</v>
       </c>
       <c r="E107" s="8"/>
@@ -13160,7 +13164,7 @@
       <c r="A13" s="11" t="s">
         <v>732</v>
       </c>
-      <c r="B13" s="51" t="s">
+      <c r="B13" s="50" t="s">
         <v>733</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -13194,7 +13198,7 @@
       <c r="A15" s="11" t="s">
         <v>735</v>
       </c>
-      <c r="B15" s="51" t="s">
+      <c r="B15" s="50" t="s">
         <v>167</v>
       </c>
       <c r="C15" s="11" t="s">
@@ -13296,7 +13300,7 @@
       <c r="A21" s="11" t="s">
         <v>729</v>
       </c>
-      <c r="B21" s="51" t="s">
+      <c r="B21" s="50" t="s">
         <v>730</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -13361,13 +13365,13 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="38" t="s">
         <v>1059</v>
       </c>
-      <c r="B25" s="39" t="s">
+      <c r="B25" s="38" t="s">
         <v>189</v>
       </c>
-      <c r="C25" s="39" t="s">
+      <c r="C25" s="38" t="s">
         <v>1060</v>
       </c>
       <c r="D25" s="19" t="s">
@@ -13378,13 +13382,13 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="39" t="s">
+      <c r="A26" s="38" t="s">
         <v>764</v>
       </c>
-      <c r="B26" s="39" t="s">
+      <c r="B26" s="38" t="s">
         <v>189</v>
       </c>
-      <c r="C26" s="39" t="s">
+      <c r="C26" s="38" t="s">
         <v>1061</v>
       </c>
       <c r="D26" s="19" t="s">
@@ -13673,7 +13677,7 @@
       <c r="B43" s="11" t="s">
         <v>1045</v>
       </c>
-      <c r="C43" s="39" t="s">
+      <c r="C43" s="38" t="s">
         <v>1085</v>
       </c>
       <c r="D43" s="11" t="s">
@@ -13792,7 +13796,7 @@
       <c r="B50" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="C50" s="39" t="s">
+      <c r="C50" s="38" t="s">
         <v>1086</v>
       </c>
       <c r="D50" s="11" t="s">
@@ -13962,7 +13966,7 @@
       <c r="B60" s="11" t="s">
         <v>728</v>
       </c>
-      <c r="C60" s="39" t="s">
+      <c r="C60" s="38" t="s">
         <v>1039</v>
       </c>
       <c r="D60" s="11" t="s">
@@ -14215,290 +14219,290 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="48" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="48" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="48" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="48" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="48" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="49" t="s">
+      <c r="A7" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="48" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="48" t="s">
         <v>95</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="48" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="49" t="s">
+      <c r="A9" s="48" t="s">
         <v>106</v>
       </c>
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="48" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="48" t="s">
         <v>118</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="48" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="48" t="s">
         <v>129</v>
       </c>
-      <c r="B11" s="49" t="s">
+      <c r="B11" s="48" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="49" t="s">
+      <c r="A12" s="48" t="s">
         <v>129</v>
       </c>
-      <c r="B12" s="49" t="s">
+      <c r="B12" s="48" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="49" t="s">
+      <c r="A13" s="48" t="s">
         <v>137</v>
       </c>
-      <c r="B13" s="49" t="s">
+      <c r="B13" s="48" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="49" t="s">
+      <c r="A14" s="48" t="s">
         <v>149</v>
       </c>
-      <c r="B14" s="49" t="s">
+      <c r="B14" s="48" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="49" t="s">
+      <c r="A15" s="48" t="s">
         <v>149</v>
       </c>
-      <c r="B15" s="49" t="s">
+      <c r="B15" s="48" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="48" t="s">
         <v>156</v>
       </c>
-      <c r="B16" s="49" t="s">
+      <c r="B16" s="48" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="49" t="s">
+      <c r="A17" s="48" t="s">
         <v>162</v>
       </c>
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="48" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="49" t="s">
+      <c r="A18" s="48" t="s">
         <v>177</v>
       </c>
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="48" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="49" t="s">
+      <c r="A19" s="48" t="s">
         <v>183</v>
       </c>
-      <c r="B19" s="49" t="s">
+      <c r="B19" s="48" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="49" t="s">
+      <c r="A20" s="48" t="s">
         <v>195</v>
       </c>
-      <c r="B20" s="49" t="s">
+      <c r="B20" s="48" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="49" t="s">
+      <c r="A21" s="48" t="s">
         <v>216</v>
       </c>
-      <c r="B21" s="49" t="s">
+      <c r="B21" s="48" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="49" t="s">
+      <c r="A22" s="48" t="s">
         <v>216</v>
       </c>
-      <c r="B22" s="49" t="s">
+      <c r="B22" s="48" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="49" t="s">
+      <c r="A23" s="48" t="s">
         <v>225</v>
       </c>
-      <c r="B23" s="49" t="s">
+      <c r="B23" s="48" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="49" t="s">
+      <c r="A24" s="48" t="s">
         <v>235</v>
       </c>
-      <c r="B24" s="49" t="s">
+      <c r="B24" s="48" t="s">
         <v>1058</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="49" t="s">
+      <c r="A25" s="48" t="s">
         <v>241</v>
       </c>
-      <c r="B25" s="49" t="s">
+      <c r="B25" s="48" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" s="49" t="s">
+      <c r="A26" s="48" t="s">
         <v>246</v>
       </c>
-      <c r="B26" s="49" t="s">
+      <c r="B26" s="48" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" s="49" t="s">
+      <c r="A27" s="48" t="s">
         <v>283</v>
       </c>
-      <c r="B27" s="49" t="s">
+      <c r="B27" s="48" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" s="49" t="s">
+      <c r="A28" s="48" t="s">
         <v>295</v>
       </c>
-      <c r="B28" s="49" t="s">
+      <c r="B28" s="48" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" s="49" t="s">
+      <c r="A29" s="48" t="s">
         <v>311</v>
       </c>
-      <c r="B29" s="49" t="s">
+      <c r="B29" s="48" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" s="49" t="s">
+      <c r="A30" s="48" t="s">
         <v>327</v>
       </c>
-      <c r="B30" s="49" t="s">
+      <c r="B30" s="48" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" s="49" t="s">
+      <c r="A31" s="48" t="s">
         <v>333</v>
       </c>
-      <c r="B31" s="49" t="s">
+      <c r="B31" s="48" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" s="49" t="s">
+      <c r="A32" s="48" t="s">
         <v>333</v>
       </c>
-      <c r="B32" s="49" t="s">
+      <c r="B32" s="48" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="49" t="s">
+      <c r="A33" s="48" t="s">
         <v>351</v>
       </c>
-      <c r="B33" s="49" t="s">
+      <c r="B33" s="48" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" s="49" t="s">
+      <c r="A34" s="48" t="s">
         <v>356</v>
       </c>
-      <c r="B34" s="49" t="s">
+      <c r="B34" s="48" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" s="49" t="s">
+      <c r="A35" s="48" t="s">
         <v>370</v>
       </c>
-      <c r="B35" s="49" t="s">
+      <c r="B35" s="48" t="s">
         <v>369</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" s="49" t="s">
+      <c r="A36" s="48" t="s">
         <v>380</v>
       </c>
-      <c r="B36" s="49" t="s">
+      <c r="B36" s="48" t="s">
         <v>386</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" s="49" t="s">
+      <c r="A37" s="48" t="s">
         <v>390</v>
       </c>
-      <c r="B37" s="49" t="s">
+      <c r="B37" s="48" t="s">
         <v>100</v>
       </c>
     </row>
@@ -14941,7 +14945,7 @@
       <c r="B38" s="11" t="s">
         <v>758</v>
       </c>
-      <c r="C38" s="47" t="s">
+      <c r="C38" s="46" t="s">
         <v>759</v>
       </c>
     </row>
@@ -15029,7 +15033,7 @@
       <c r="B46" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="C46" s="39" t="s">
+      <c r="C46" s="38" t="s">
         <v>821</v>
       </c>
     </row>
@@ -15150,7 +15154,7 @@
       <c r="B57" s="11" t="s">
         <v>898</v>
       </c>
-      <c r="C57" s="48" t="s">
+      <c r="C57" s="47" t="s">
         <v>899</v>
       </c>
     </row>
@@ -15672,7 +15676,7 @@
       <c r="B22" s="11" t="s">
         <v>1055</v>
       </c>
-      <c r="C22" s="39" t="s">
+      <c r="C22" s="38" t="s">
         <v>471</v>
       </c>
       <c r="D22" s="11" t="s">
@@ -15833,200 +15837,200 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23046875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.23046875" style="45" customWidth="1"/>
-    <col min="2" max="2" width="14.4609375" style="45" customWidth="1"/>
-    <col min="3" max="3" width="35.4609375" style="45" customWidth="1"/>
-    <col min="4" max="4" width="38" style="45" customWidth="1"/>
-    <col min="5" max="5" width="15.07421875" style="45" customWidth="1"/>
-    <col min="6" max="16384" width="9.23046875" style="45"/>
+    <col min="1" max="1" width="14.23046875" style="44" customWidth="1"/>
+    <col min="2" max="2" width="14.4609375" style="44" customWidth="1"/>
+    <col min="3" max="3" width="35.4609375" style="44" customWidth="1"/>
+    <col min="4" max="4" width="38" style="44" customWidth="1"/>
+    <col min="5" max="5" width="15.07421875" style="44" customWidth="1"/>
+    <col min="6" max="16384" width="9.23046875" style="44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:4" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="45" t="s">
         <v>1083</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="45" t="s">
         <v>631</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="45" t="s">
         <v>632</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="44" t="s">
         <v>996</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="44" t="s">
         <v>987</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="44" t="s">
         <v>988</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="44" t="s">
         <v>989</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="44" t="s">
         <v>638</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="44" t="s">
         <v>997</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="44" t="s">
         <v>998</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="44" t="s">
         <v>990</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="44" t="s">
         <v>647</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="44" t="s">
         <v>991</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="44" t="s">
         <v>908</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="44" t="s">
         <v>981</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="44" t="s">
         <v>982</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="44" t="s">
         <v>824</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="44" t="s">
         <v>979</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="44" t="s">
         <v>980</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="44" t="s">
         <v>133</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="D8" s="45" t="s">
+      <c r="D8" s="44" t="s">
         <v>986</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="44" t="s">
         <v>983</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="44" t="s">
         <v>984</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="44" t="s">
         <v>985</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="44" t="s">
         <v>983</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="44" t="s">
         <v>992</v>
       </c>
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="44" t="s">
         <v>993</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="44" t="s">
         <v>1001</v>
       </c>
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="44" t="s">
         <v>1002</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="44" t="s">
         <v>1003</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="44" t="s">
         <v>656</v>
       </c>
-      <c r="B12" s="45" t="s">
+      <c r="B12" s="44" t="s">
         <v>994</v>
       </c>
-      <c r="C12" s="45" t="s">
+      <c r="C12" s="44" t="s">
         <v>995</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="44" t="s">
         <v>1053</v>
       </c>
-      <c r="B13" s="45" t="s">
+      <c r="B13" s="44" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="46" t="s">
+      <c r="A19" s="45" t="s">
         <v>900</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="45" t="s">
+      <c r="A20" s="44" t="s">
         <v>646</v>
       </c>
-      <c r="B20" s="45" t="s">
+      <c r="B20" s="44" t="s">
         <v>999</v>
       </c>
-      <c r="D20" s="45" t="s">
+      <c r="D20" s="44" t="s">
         <v>1000</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="45" t="s">
+      <c r="A21" s="44" t="s">
         <v>1001</v>
       </c>
-      <c r="B21" s="45" t="s">
+      <c r="B21" s="44" t="s">
         <v>1002</v>
       </c>
-      <c r="D21" s="45" t="s">
+      <c r="D21" s="44" t="s">
         <v>1003</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="45" t="s">
+      <c r="A22" s="44" t="s">
         <v>764</v>
       </c>
-      <c r="B22" s="45" t="s">
+      <c r="B22" s="44" t="s">
         <v>1004</v>
       </c>
-      <c r="D22" s="45" t="s">
+      <c r="D22" s="44" t="s">
         <v>1005</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="45" t="s">
+      <c r="A23" s="44" t="s">
         <v>1006</v>
       </c>
-      <c r="B23" s="45" t="s">
+      <c r="B23" s="44" t="s">
         <v>1007</v>
       </c>
-      <c r="D23" s="45" t="s">
+      <c r="D23" s="44" t="s">
         <v>1008</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update January and February newsletters; correct typos and add residents directory
</commit_message>
<xml_diff>
--- a/3-1-heritage/0-heritage-happenings/2025/02-february-hh/residents-directory/2025-02-heritage-resident-directory.xlsx
+++ b/3-1-heritage/0-heritage-happenings/2025/02-february-hh/residents-directory/2025-02-heritage-resident-directory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4348e1419f457eb2/Documents/GitHub/theo-armour-agenda/3-1-heritage/0-heritage-happenings/2025/02-february-hh/residents-directory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="807" documentId="8_{47523533-A004-48EF-BEEC-0FA3DE3C4717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E43E5195-7A6B-47B0-9017-E87EB37E4A41}"/>
+  <xr:revisionPtr revIDLastSave="828" documentId="8_{47523533-A004-48EF-BEEC-0FA3DE3C4717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F79F4AC5-A7DA-4B78-8AED-D5D5063AD662}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="754" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="754" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="residents" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1678" uniqueCount="1092">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1690" uniqueCount="1100">
   <si>
     <t>First Name</t>
   </si>
@@ -3346,6 +3346,30 @@
   </si>
   <si>
     <t>Light Blue: Departed or deceased</t>
+  </si>
+  <si>
+    <t>Sinclair</t>
+  </si>
+  <si>
+    <t>patricksinclair@yahoo.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karen </t>
+  </si>
+  <si>
+    <t>Art Class</t>
+  </si>
+  <si>
+    <t>zukorart@sbcglobal.net</t>
+  </si>
+  <si>
+    <t>Maria</t>
+  </si>
+  <si>
+    <t>Church</t>
+  </si>
+  <si>
+    <t>Art for Elders</t>
   </si>
 </sst>
 </file>
@@ -9728,7 +9752,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26C4F1CA-A107-47E1-B61D-684F7BB5060E}">
   <dimension ref="A1:Z173"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" showRuler="0" view="pageLayout" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" showZeros="0" showRuler="0" view="pageLayout" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
@@ -12305,9 +12329,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6607607A-1D03-4DF1-ADDE-DAB7CE4E5761}">
   <dimension ref="A1:B76"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -16045,11 +16067,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5C4CAD2-851C-4D78-8B2D-D5100B32C514}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23046875" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -16063,7 +16085,7 @@
     <col min="7" max="16384" width="9.23046875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>1083</v>
       </c>
@@ -16080,20 +16102,60 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>1090</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="F2" s="11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="11" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="11" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>1098</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>1074</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>1092</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>1093</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="11" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>667</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>